<commit_message>
Added calculation by temperature
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>9.52</v>
+        <v>10.8</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -542,7 +542,7 @@
         <v>0.31</v>
       </c>
       <c r="G5" t="n">
-        <v>9.757999999999999</v>
+        <v>7.8503232</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -749,7 +749,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.15</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>8.889999999999999</v>
+        <v>2.53</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1133,7 +1133,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>6.284000000000001</v>
+        <v>11.536</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -2786,7 +2786,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.6360000000000001</v>
+        <v>0.68</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3255,7 +3255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H49"/>
+  <dimension ref="B2:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H5"/>
@@ -3346,7 +3346,7 @@
         <v>0.01</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5082000000000002</v>
+        <v>0</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -3538,6 +3538,244 @@
         <v>18.04</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B2:H49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="10.44140625" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>m3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">k = </t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>t/m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Вы ввели:</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Результат:</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8150000000000001</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.672</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>t</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="1" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="1" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="1" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="1" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="1" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="1" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>2.52</v>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
     <row r="29"/>
     <row r="30"/>
     <row r="31"/>
@@ -3564,227 +3802,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="B2:H20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="10.44140625" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">k = </t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>t/m3</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Вы ввели:</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Результат:</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>m3</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="1" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="1" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="1" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="1" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="1" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>1.49</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="1" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="1" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" s="1" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1.93</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" s="1" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>2.08</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="1" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>2.23</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="1" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="1" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>2.52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -3842,7 +3859,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3863,7 +3880,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.8150000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3879,7 +3896,7 @@
         <v>0.3</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6846</v>
+        <v>0.7721192640000001</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -4069,7 +4086,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4090,7 +4107,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.668</v>
+        <v>2.932</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4106,7 +4123,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>2.24112</v>
+        <v>0.48048</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -4384,7 +4401,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.22</v>
+        <v>0.55</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4405,7 +4422,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.824</v>
+        <v>2.602</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4699,7 +4716,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.99</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4720,7 +4737,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.3100000000000001</v>
+        <v>0.554</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4985,7 +5002,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -5006,7 +5023,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.5140000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
New tab and summary
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>9.199999999999999</v>
+        <v>7.71</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -776,7 +776,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.53</v>
+        <v>1.71</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.12</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>8.482000000000001</v>
+        <v>1.71</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1793,7 +1793,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.23</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1814,7 +1814,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.36</v>
+        <v>0.068</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2068,7 +2068,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -2089,7 +2089,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.08</v>
+        <v>0.27</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.23</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -2361,7 +2361,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.39</v>
+        <v>0.538</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2531,7 +2531,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>1.35</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -2552,7 +2552,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.165</v>
+        <v>0.14</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -2798,7 +2798,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -2819,7 +2819,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.68</v>
+        <v>0.57</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3064,7 +3064,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3085,7 +3085,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.79</v>
+        <v>1.35</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3363,7 +3363,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.6050000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3636,7 +3636,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.8150000000000001</v>
+        <v>1.16</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3863,7 +3863,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3884,7 +3884,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.74</v>
+        <v>1.16</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4090,7 +4090,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4111,7 +4111,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.602</v>
+        <v>2.29</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4405,7 +4405,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4426,7 +4426,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.602</v>
+        <v>2.29</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4720,7 +4720,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.99</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4741,7 +4741,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.554</v>
+        <v>0.438</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -5006,7 +5006,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.55</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -5027,7 +5027,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.5050000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Generate report was added
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H49"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B21"/>
@@ -686,33 +686,6 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
@@ -1793,7 +1766,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1814,7 +1787,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.068</v>
+        <v>0.08</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3064,7 +3037,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3085,7 +3058,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.35</v>
+        <v>3.29</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3288,7 +3261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H28"/>
+  <dimension ref="B2:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:H5"/>
@@ -3342,7 +3315,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3363,7 +3336,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0.39</v>
+        <v>0.82</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -3571,6 +3544,27 @@
         <v>18.04</v>
       </c>
     </row>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3636,7 +3630,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.78</v>
+        <v>0.2</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -3657,7 +3651,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>1.16</v>
+        <v>0.3</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -4090,7 +4084,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -4111,7 +4105,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2.29</v>
+        <v>0.954</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
New features were added
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -449,13 +449,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="10.88671875" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="6" max="6"/>
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>14.22</v>
+        <v>16.035</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -542,7 +542,7 @@
         <v>0.31</v>
       </c>
       <c r="G5" t="n">
-        <v>7.8503232</v>
+        <v>15.57344856</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -686,6 +686,33 @@
         <v>29</v>
       </c>
     </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" verticalDpi="0"/>
@@ -2989,7 +3016,7 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="11.21875" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3267,7 +3294,7 @@
       <selection activeCell="B2" sqref="B2:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="12.21875" customWidth="1" min="6" max="6"/>
   </cols>
@@ -3561,7 +3588,7 @@
       <selection activeCell="D3" sqref="D3:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="10.44140625" customWidth="1" min="6" max="6"/>
   </cols>
@@ -4327,7 +4354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:H49"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
@@ -4631,24 +4658,6 @@
         <v>11.62</v>
       </c>
     </row>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>